<commit_message>
Other division cable schedule completed
</commit_message>
<xml_diff>
--- a/thermax_backend/templates/heating_cable_schedule_template.xlsx
+++ b/thermax_backend/templates/heating_cable_schedule_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\abhishekraje30\frappe-bench\apps\thermax_backend\thermax_backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931B1DCF-761D-4B0A-BFB1-E45253EE2091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72AC1FB-877A-4D17-BD6C-59747696C503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{D4E0A742-FDEC-4788-85D8-458011EB4DFD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D4E0A742-FDEC-4788-85D8-458011EB4DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="COVER" sheetId="2" r:id="rId1"/>
@@ -805,6 +805,57 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -840,57 +891,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -901,6 +901,14 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -930,14 +938,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1430,7 +1430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BE4FFA-FAC3-4B5C-8E7B-B7CD9E0BEF6B}">
   <dimension ref="A1:CD35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
@@ -2079,50 +2079,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50"/>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="52"/>
+      <c r="A1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="55"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="23.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="46"/>
     </row>
     <row r="4" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="61"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="49"/>
     </row>
     <row r="5" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
@@ -2136,76 +2136,76 @@
     </row>
     <row r="6" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="64" t="s">
+      <c r="C6" s="51"/>
+      <c r="D6" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="66"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="54"/>
       <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="59"/>
       <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="42"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59"/>
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="42"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
       <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="42"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
       <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="16"/>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="47"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="64"/>
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" s="21" customFormat="1" ht="15.5" x14ac:dyDescent="0.3">
@@ -2469,12 +2469,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G6"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:G10"/>
     <mergeCell ref="B11:C11"/>
@@ -2485,6 +2479,12 @@
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:G9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2495,33 +2495,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77278457-2AA5-4395-885E-2416C9B7D6AE}">
   <dimension ref="A1:BM11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="A1:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6328125" customWidth="1"/>
+    <col min="18" max="18" width="20.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:65" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="78"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="70"/>
       <c r="S1" s="2"/>
       <c r="T1" s="3"/>
       <c r="U1" s="2"/>
@@ -2998,25 +3016,25 @@
     </row>
     <row r="8" spans="1:65" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="70"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="72"/>
       <c r="S8" s="2"/>
       <c r="T8" s="3"/>
       <c r="U8" s="2"/>
@@ -3066,38 +3084,38 @@
       <c r="BM8" s="2"/>
     </row>
     <row r="9" spans="1:65" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="73" t="s">
+      <c r="E9" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="73" t="s">
+      <c r="F9" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="75" t="s">
+      <c r="G9" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="77"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
-      <c r="R9" s="76" t="s">
+      <c r="R9" s="78" t="s">
         <v>15</v>
       </c>
       <c r="S9" s="2"/>
@@ -3148,13 +3166,13 @@
       <c r="BL9" s="2"/>
       <c r="BM9" s="2"/>
     </row>
-    <row r="10" spans="1:65" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="71"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
+    <row r="10" spans="1:65" s="11" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="73"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
       <c r="G10" s="9" t="s">
         <v>16</v>
       </c>
@@ -3188,7 +3206,7 @@
       <c r="Q10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="R10" s="76"/>
+      <c r="R10" s="78"/>
       <c r="S10" s="10"/>
       <c r="T10" s="3"/>
       <c r="U10" s="10"/>
@@ -3260,12 +3278,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B6:R6"/>
-    <mergeCell ref="B1:R1"/>
-    <mergeCell ref="B2:R2"/>
-    <mergeCell ref="B3:R3"/>
-    <mergeCell ref="B4:R4"/>
-    <mergeCell ref="B5:R5"/>
     <mergeCell ref="B7:R7"/>
     <mergeCell ref="B8:R8"/>
     <mergeCell ref="A9:A10"/>
@@ -3276,6 +3288,12 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:N9"/>
     <mergeCell ref="R9:R10"/>
+    <mergeCell ref="B6:R6"/>
+    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="B3:R3"/>
+    <mergeCell ref="B4:R4"/>
+    <mergeCell ref="B5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3290,15 +3308,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9548EEE6D3B14BA64FE13261469485" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="731c574389bf7010e1fd83ba65962491">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7b113091-3911-42e5-9d43-1d1d14e29103" xmlns:ns4="79d5e28a-71b7-4357-9555-ecca6070aec6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2da99a392d92fb994d61b1b6d5532d6" ns3:_="" ns4:_="">
     <xsd:import namespace="7b113091-3911-42e5-9d43-1d1d14e29103"/>
@@ -3545,6 +3554,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F0DD04F-2B90-4C86-8F24-95174DAB3E88}">
   <ds:schemaRefs>
@@ -3563,14 +3581,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB7A903-82F2-4FE7-8BAF-E1293493477E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73785DB6-09FE-45D1-9A04-A19A00D2F848}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3587,4 +3597,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB7A903-82F2-4FE7-8BAF-E1293493477E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>